<commit_message>
readValue column check if set to 1 mean this key should be value store in db
</commit_message>
<xml_diff>
--- a/ReadPcap_InJsonForma_EntryFromExcel/ConsoleApp3/sample_data.xlsx
+++ b/ReadPcap_InJsonForma_EntryFromExcel/ConsoleApp3/sample_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OLD\Kavoshcom\MNM group\MCI R&amp;D Probe\KPI and Events\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\L3Mess\Z_Final_ReadJson\ReadPcap_InJsonForma_EntryFromExcel\ConsoleApp3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1659,7 +1659,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1667,7 +1667,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1687,7 +1687,7 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2039,22 +2039,22 @@
   <dimension ref="A1:F268"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <pane ySplit="1" topLeftCell="A256" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E105" sqref="E105:E110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.625" customWidth="1"/>
-    <col min="2" max="2" width="32.75" customWidth="1"/>
-    <col min="3" max="3" width="40.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.125" customWidth="1"/>
+    <col min="1" max="1" width="44.6328125" customWidth="1"/>
+    <col min="2" max="2" width="32.7265625" customWidth="1"/>
+    <col min="3" max="3" width="40.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.08984375" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="7" width="22.375" customWidth="1"/>
+    <col min="7" max="7" width="22.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2074,79 +2074,95 @@
         <v>365</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>250</v>
       </c>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>437</v>
       </c>
       <c r="C3" t="s">
         <v>252</v>
       </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>253</v>
       </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>399</v>
       </c>
       <c r="C5" t="s">
         <v>529</v>
       </c>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>400</v>
       </c>
       <c r="C6" t="s">
         <v>254</v>
       </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>401</v>
       </c>
       <c r="C7" t="s">
         <v>255</v>
       </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>402</v>
       </c>
       <c r="C8" t="s">
         <v>256</v>
       </c>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>403</v>
       </c>
       <c r="C9" t="s">
         <v>257</v>
       </c>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>438</v>
       </c>
@@ -2156,9 +2172,11 @@
       <c r="C10" t="s">
         <v>258</v>
       </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>439</v>
       </c>
@@ -2168,9 +2186,11 @@
       <c r="C11" t="s">
         <v>259</v>
       </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>440</v>
       </c>
@@ -2180,9 +2200,11 @@
       <c r="C12" t="s">
         <v>406</v>
       </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>446</v>
       </c>
@@ -2192,9 +2214,11 @@
       <c r="C13" t="s">
         <v>374</v>
       </c>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>447</v>
       </c>
@@ -2204,9 +2228,11 @@
       <c r="C14" t="s">
         <v>406</v>
       </c>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>448</v>
       </c>
@@ -2216,9 +2242,11 @@
       <c r="C15" t="s">
         <v>259</v>
       </c>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E15" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -2228,63 +2256,77 @@
       <c r="C16" t="s">
         <v>377</v>
       </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>449</v>
       </c>
       <c r="C17" t="s">
         <v>378</v>
       </c>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>450</v>
       </c>
       <c r="C18" t="s">
         <v>379</v>
       </c>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>451</v>
       </c>
       <c r="C19" t="s">
         <v>380</v>
       </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>452</v>
       </c>
       <c r="C20" t="s">
         <v>381</v>
       </c>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>453</v>
       </c>
       <c r="C21" t="s">
         <v>382</v>
       </c>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>454</v>
       </c>
       <c r="C22" t="s">
         <v>383</v>
       </c>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2294,9 +2336,11 @@
       <c r="C23" t="s">
         <v>376</v>
       </c>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>527</v>
       </c>
@@ -2307,7 +2351,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -2315,7 +2359,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>458</v>
       </c>
@@ -2326,7 +2370,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>459</v>
       </c>
@@ -2337,7 +2381,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>523</v>
       </c>
@@ -2348,7 +2392,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>524</v>
       </c>
@@ -2359,16 +2403,18 @@
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>6</v>
       </c>
       <c r="C30" t="s">
         <v>522</v>
       </c>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E30" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>528</v>
       </c>
@@ -2378,9 +2424,11 @@
       <c r="C31" t="s">
         <v>387</v>
       </c>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E31" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>525</v>
       </c>
@@ -2390,9 +2438,11 @@
       <c r="C32" t="s">
         <v>388</v>
       </c>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E32" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>442</v>
       </c>
@@ -2400,7 +2450,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>443</v>
       </c>
@@ -2408,7 +2458,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>444</v>
       </c>
@@ -2416,7 +2466,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>445</v>
       </c>
@@ -2424,7 +2474,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -2432,7 +2482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2440,7 +2490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -2448,16 +2498,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>14</v>
       </c>
       <c r="C40" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E40" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>518</v>
       </c>
@@ -2467,9 +2519,11 @@
       <c r="C41" t="s">
         <v>389</v>
       </c>
-      <c r="E41" s="6"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E41" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>519</v>
       </c>
@@ -2479,9 +2533,11 @@
       <c r="C42" t="s">
         <v>390</v>
       </c>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E42" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>520</v>
       </c>
@@ -2491,9 +2547,11 @@
       <c r="C43" t="s">
         <v>391</v>
       </c>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E43" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>521</v>
       </c>
@@ -2503,9 +2561,11 @@
       <c r="C44" t="s">
         <v>392</v>
       </c>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E44" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -2513,7 +2573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -2521,7 +2581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -2529,7 +2589,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>22</v>
       </c>
@@ -2537,7 +2597,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -2545,7 +2605,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -2553,7 +2613,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>28</v>
       </c>
@@ -2561,7 +2621,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>30</v>
       </c>
@@ -2569,7 +2629,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>32</v>
       </c>
@@ -2577,7 +2637,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>34</v>
       </c>
@@ -2585,7 +2645,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -2593,7 +2653,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>38</v>
       </c>
@@ -2601,7 +2661,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>40</v>
       </c>
@@ -2609,7 +2669,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -2617,7 +2677,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>44</v>
       </c>
@@ -2625,7 +2685,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>46</v>
       </c>
@@ -2633,7 +2693,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -2641,7 +2701,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>50</v>
       </c>
@@ -2649,7 +2709,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>52</v>
       </c>
@@ -2657,7 +2717,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>247</v>
       </c>
@@ -2665,7 +2725,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>248</v>
       </c>
@@ -2673,7 +2733,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>249</v>
       </c>
@@ -2681,16 +2741,18 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>56</v>
       </c>
       <c r="C67" t="s">
         <v>260</v>
       </c>
-      <c r="E67" s="6"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E67" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>58</v>
       </c>
@@ -2698,7 +2760,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>60</v>
       </c>
@@ -2706,16 +2768,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>62</v>
       </c>
       <c r="C70" t="s">
         <v>61</v>
       </c>
-      <c r="E70" s="6"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E70" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>412</v>
       </c>
@@ -2726,9 +2790,11 @@
         <v>530</v>
       </c>
       <c r="D71" s="2"/>
-      <c r="E71" s="6"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E71" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>413</v>
       </c>
@@ -2738,9 +2804,11 @@
       <c r="C72" t="s">
         <v>531</v>
       </c>
-      <c r="E72" s="6"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E72" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>414</v>
       </c>
@@ -2751,9 +2819,11 @@
         <v>532</v>
       </c>
       <c r="D73" s="2"/>
-      <c r="E73" s="6"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E73" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>415</v>
       </c>
@@ -2764,9 +2834,11 @@
         <v>261</v>
       </c>
       <c r="D74" s="2"/>
-      <c r="E74" s="6"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E74" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>416</v>
       </c>
@@ -2777,9 +2849,11 @@
         <v>262</v>
       </c>
       <c r="D75" s="2"/>
-      <c r="E75" s="6"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E75" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>412</v>
       </c>
@@ -2790,9 +2864,11 @@
         <v>419</v>
       </c>
       <c r="D76" s="2"/>
-      <c r="E76" s="6"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E76" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>413</v>
       </c>
@@ -2803,9 +2879,11 @@
         <v>420</v>
       </c>
       <c r="D77" s="2"/>
-      <c r="E77" s="6"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E77" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>414</v>
       </c>
@@ -2816,9 +2894,11 @@
         <v>421</v>
       </c>
       <c r="D78" s="2"/>
-      <c r="E78" s="6"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E78" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>415</v>
       </c>
@@ -2829,9 +2909,11 @@
         <v>261</v>
       </c>
       <c r="D79" s="2"/>
-      <c r="E79" s="6"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E79" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>422</v>
       </c>
@@ -2841,9 +2923,11 @@
       <c r="C80" t="s">
         <v>394</v>
       </c>
-      <c r="E80" s="6"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E80" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>423</v>
       </c>
@@ -2853,9 +2937,11 @@
       <c r="C81" t="s">
         <v>395</v>
       </c>
-      <c r="E81" s="6"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E81" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>424</v>
       </c>
@@ -2865,9 +2951,11 @@
       <c r="C82" t="s">
         <v>396</v>
       </c>
-      <c r="E82" s="6"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E82" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>425</v>
       </c>
@@ -2877,9 +2965,11 @@
       <c r="C83" t="s">
         <v>397</v>
       </c>
-      <c r="E83" s="6"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E83" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>426</v>
       </c>
@@ -2889,9 +2979,11 @@
       <c r="C84" t="s">
         <v>393</v>
       </c>
-      <c r="E84" s="6"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E84" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>481</v>
       </c>
@@ -2904,7 +2996,7 @@
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>510</v>
       </c>
@@ -2917,7 +3009,7 @@
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>511</v>
       </c>
@@ -2930,7 +3022,7 @@
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>482</v>
       </c>
@@ -2943,7 +3035,7 @@
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>483</v>
       </c>
@@ -2956,7 +3048,7 @@
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>484</v>
       </c>
@@ -2969,7 +3061,7 @@
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>485</v>
       </c>
@@ -2982,7 +3074,7 @@
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>486</v>
       </c>
@@ -2995,7 +3087,7 @@
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>487</v>
       </c>
@@ -3008,7 +3100,7 @@
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>488</v>
       </c>
@@ -3021,7 +3113,7 @@
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>489</v>
       </c>
@@ -3034,7 +3126,7 @@
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>490</v>
       </c>
@@ -3047,7 +3139,7 @@
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>491</v>
       </c>
@@ -3060,7 +3152,7 @@
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>492</v>
       </c>
@@ -3073,7 +3165,7 @@
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>493</v>
       </c>
@@ -3086,7 +3178,7 @@
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>494</v>
       </c>
@@ -3099,7 +3191,7 @@
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>64</v>
       </c>
@@ -3107,7 +3199,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>66</v>
       </c>
@@ -3115,7 +3207,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>68</v>
       </c>
@@ -3123,7 +3215,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>70</v>
       </c>
@@ -3131,7 +3223,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>512</v>
       </c>
@@ -3141,9 +3233,11 @@
       <c r="C105" t="s">
         <v>433</v>
       </c>
-      <c r="E105" s="6"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E105" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>513</v>
       </c>
@@ -3153,9 +3247,11 @@
       <c r="C106" t="s">
         <v>432</v>
       </c>
-      <c r="E106" s="6"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E106" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>514</v>
       </c>
@@ -3165,9 +3261,11 @@
       <c r="C107" t="s">
         <v>431</v>
       </c>
-      <c r="E107" s="6"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E107" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>515</v>
       </c>
@@ -3177,9 +3275,11 @@
       <c r="C108" t="s">
         <v>430</v>
       </c>
-      <c r="E108" s="6"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E108" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>516</v>
       </c>
@@ -3189,9 +3289,11 @@
       <c r="C109" t="s">
         <v>429</v>
       </c>
-      <c r="E109" s="6"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E109" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>517</v>
       </c>
@@ -3201,9 +3303,11 @@
       <c r="C110" t="s">
         <v>428</v>
       </c>
-      <c r="E110" s="6"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E110" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>72</v>
       </c>
@@ -3211,7 +3315,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>74</v>
       </c>
@@ -3222,7 +3326,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>76</v>
       </c>
@@ -3230,7 +3334,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>78</v>
       </c>
@@ -3241,7 +3345,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>80</v>
       </c>
@@ -3249,7 +3353,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>81</v>
       </c>
@@ -3260,7 +3364,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>82</v>
       </c>
@@ -3271,7 +3375,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>83</v>
       </c>
@@ -3282,7 +3386,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>84</v>
       </c>
@@ -3293,7 +3397,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>85</v>
       </c>
@@ -3304,7 +3408,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>86</v>
       </c>
@@ -3315,7 +3419,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>87</v>
       </c>
@@ -3326,7 +3430,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>88</v>
       </c>
@@ -3337,7 +3441,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>89</v>
       </c>
@@ -3348,7 +3452,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>90</v>
       </c>
@@ -3359,7 +3463,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>91</v>
       </c>
@@ -3370,7 +3474,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>92</v>
       </c>
@@ -3381,7 +3485,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>93</v>
       </c>
@@ -3392,7 +3496,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>94</v>
       </c>
@@ -3403,7 +3507,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>95</v>
       </c>
@@ -3414,7 +3518,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>96</v>
       </c>
@@ -3425,7 +3529,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>97</v>
       </c>
@@ -3436,7 +3540,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>98</v>
       </c>
@@ -3447,7 +3551,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>99</v>
       </c>
@@ -3458,7 +3562,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>100</v>
       </c>
@@ -3469,7 +3573,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>101</v>
       </c>
@@ -3480,7 +3584,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>102</v>
       </c>
@@ -3491,7 +3595,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>103</v>
       </c>
@@ -3502,7 +3606,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>104</v>
       </c>
@@ -3513,7 +3617,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>105</v>
       </c>
@@ -3524,7 +3628,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>106</v>
       </c>
@@ -3535,7 +3639,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>107</v>
       </c>
@@ -3546,7 +3650,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>108</v>
       </c>
@@ -3557,7 +3661,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>109</v>
       </c>
@@ -3568,7 +3672,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>110</v>
       </c>
@@ -3579,7 +3683,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>111</v>
       </c>
@@ -3590,7 +3694,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>112</v>
       </c>
@@ -3601,7 +3705,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>113</v>
       </c>
@@ -3612,7 +3716,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>114</v>
       </c>
@@ -3623,7 +3727,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>115</v>
       </c>
@@ -3634,7 +3738,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>116</v>
       </c>
@@ -3645,7 +3749,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>117</v>
       </c>
@@ -3656,7 +3760,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>118</v>
       </c>
@@ -3667,7 +3771,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>119</v>
       </c>
@@ -3678,7 +3782,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>120</v>
       </c>
@@ -3689,7 +3793,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>121</v>
       </c>
@@ -3700,7 +3804,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>122</v>
       </c>
@@ -3711,7 +3815,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>123</v>
       </c>
@@ -3722,7 +3826,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>124</v>
       </c>
@@ -3733,7 +3837,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>125</v>
       </c>
@@ -3744,7 +3848,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>126</v>
       </c>
@@ -3755,7 +3859,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>127</v>
       </c>
@@ -3766,7 +3870,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>128</v>
       </c>
@@ -3777,7 +3881,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>129</v>
       </c>
@@ -3788,7 +3892,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>130</v>
       </c>
@@ -3799,7 +3903,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>131</v>
       </c>
@@ -3810,7 +3914,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>132</v>
       </c>
@@ -3821,7 +3925,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>133</v>
       </c>
@@ -3832,7 +3936,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>134</v>
       </c>
@@ -3843,7 +3947,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>135</v>
       </c>
@@ -3854,7 +3958,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>136</v>
       </c>
@@ -3865,7 +3969,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>137</v>
       </c>
@@ -3876,7 +3980,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>138</v>
       </c>
@@ -3887,7 +3991,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>139</v>
       </c>
@@ -3898,7 +4002,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>140</v>
       </c>
@@ -3909,7 +4013,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>141</v>
       </c>
@@ -3920,7 +4024,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>142</v>
       </c>
@@ -3931,7 +4035,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>143</v>
       </c>
@@ -3942,7 +4046,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>144</v>
       </c>
@@ -3953,7 +4057,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>145</v>
       </c>
@@ -3964,7 +4068,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>146</v>
       </c>
@@ -3975,7 +4079,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>147</v>
       </c>
@@ -3986,7 +4090,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>148</v>
       </c>
@@ -3997,7 +4101,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>149</v>
       </c>
@@ -4008,7 +4112,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>150</v>
       </c>
@@ -4019,7 +4123,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>151</v>
       </c>
@@ -4030,7 +4134,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>152</v>
       </c>
@@ -4041,7 +4145,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>153</v>
       </c>
@@ -4052,7 +4156,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>154</v>
       </c>
@@ -4063,7 +4167,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>155</v>
       </c>
@@ -4074,7 +4178,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>156</v>
       </c>
@@ -4085,7 +4189,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>157</v>
       </c>
@@ -4096,7 +4200,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>158</v>
       </c>
@@ -4107,7 +4211,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>159</v>
       </c>
@@ -4118,7 +4222,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>161</v>
       </c>
@@ -4135,7 +4239,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>162</v>
       </c>
@@ -4152,7 +4256,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>163</v>
       </c>
@@ -4163,7 +4267,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>165</v>
       </c>
@@ -4177,7 +4281,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>166</v>
       </c>
@@ -4188,7 +4292,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>167</v>
       </c>
@@ -4199,7 +4303,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>168</v>
       </c>
@@ -4210,7 +4314,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>169</v>
       </c>
@@ -4221,7 +4325,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>170</v>
       </c>
@@ -4232,7 +4336,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>171</v>
       </c>
@@ -4243,7 +4347,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>172</v>
       </c>
@@ -4254,7 +4358,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>173</v>
       </c>
@@ -4265,7 +4369,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>174</v>
       </c>
@@ -4276,7 +4380,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>175</v>
       </c>
@@ -4287,7 +4391,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>176</v>
       </c>
@@ -4298,7 +4402,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>177</v>
       </c>
@@ -4309,7 +4413,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>178</v>
       </c>
@@ -4320,7 +4424,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>179</v>
       </c>
@@ -4331,7 +4435,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>180</v>
       </c>
@@ -4342,7 +4446,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>181</v>
       </c>
@@ -4353,7 +4457,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>182</v>
       </c>
@@ -4364,7 +4468,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>183</v>
       </c>
@@ -4375,7 +4479,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>184</v>
       </c>
@@ -4386,7 +4490,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>185</v>
       </c>
@@ -4397,7 +4501,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>186</v>
       </c>
@@ -4408,7 +4512,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>187</v>
       </c>
@@ -4419,7 +4523,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>188</v>
       </c>
@@ -4430,7 +4534,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>189</v>
       </c>
@@ -4441,7 +4545,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>190</v>
       </c>
@@ -4452,7 +4556,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>191</v>
       </c>
@@ -4463,7 +4567,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>192</v>
       </c>
@@ -4474,7 +4578,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>193</v>
       </c>
@@ -4485,7 +4589,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>194</v>
       </c>
@@ -4496,7 +4600,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>195</v>
       </c>
@@ -4507,7 +4611,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>196</v>
       </c>
@@ -4518,7 +4622,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>197</v>
       </c>
@@ -4529,7 +4633,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>198</v>
       </c>
@@ -4540,7 +4644,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>199</v>
       </c>
@@ -4551,7 +4655,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>200</v>
       </c>
@@ -4562,7 +4666,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>201</v>
       </c>
@@ -4573,7 +4677,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>202</v>
       </c>
@@ -4584,7 +4688,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>203</v>
       </c>
@@ -4595,7 +4699,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>204</v>
       </c>
@@ -4606,7 +4710,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>205</v>
       </c>
@@ -4617,7 +4721,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>206</v>
       </c>
@@ -4628,7 +4732,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>207</v>
       </c>
@@ -4639,7 +4743,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>208</v>
       </c>
@@ -4650,7 +4754,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>209</v>
       </c>
@@ -4661,7 +4765,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>210</v>
       </c>
@@ -4672,7 +4776,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>211</v>
       </c>
@@ -4683,7 +4787,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>245</v>
       </c>
@@ -4691,7 +4795,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>244</v>
       </c>
@@ -4699,7 +4803,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>212</v>
       </c>
@@ -4710,7 +4814,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>213</v>
       </c>
@@ -4721,7 +4825,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>214</v>
       </c>
@@ -4732,7 +4836,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>215</v>
       </c>
@@ -4743,7 +4847,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>398</v>
       </c>
@@ -4754,7 +4858,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>216</v>
       </c>
@@ -4765,7 +4869,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>217</v>
       </c>
@@ -4776,7 +4880,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>219</v>
       </c>
@@ -4790,7 +4894,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>221</v>
       </c>
@@ -4798,7 +4902,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>223</v>
       </c>
@@ -4806,7 +4910,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>225</v>
       </c>
@@ -4814,7 +4918,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>227</v>
       </c>
@@ -4822,7 +4926,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>229</v>
       </c>
@@ -4830,7 +4934,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>231</v>
       </c>
@@ -4838,7 +4942,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>233</v>
       </c>
@@ -4846,7 +4950,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A262" s="3" t="s">
         <v>234</v>
       </c>
@@ -4857,7 +4961,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>236</v>
       </c>
@@ -4865,7 +4969,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A264" s="3" t="s">
         <v>237</v>
       </c>
@@ -4876,7 +4980,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>238</v>
       </c>
@@ -4884,7 +4988,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A266" s="3" t="s">
         <v>239</v>
       </c>
@@ -4898,7 +5002,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>241</v>
       </c>
@@ -4906,7 +5010,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>243</v>
       </c>

</xml_diff>